<commit_message>
almost done story 1
</commit_message>
<xml_diff>
--- a/Story1/Data/IIJA FUNDING AS OF MARCH 2023.xlsx
+++ b/Story1/Data/IIJA FUNDING AS OF MARCH 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgral\Google Drive\EDU\CUNY SPS\Data 608\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2a0fcda8f0f3eb6/Documents/repos/Data608/Story1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC05A66-F486-4C56-A47B-905348F42D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2DC05A66-F486-4C56-A47B-905348F42D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C2CF55D-BD65-4280-A694-2424B6DE17EC}"/>
   <bookViews>
-    <workbookView xWindow="26805" yWindow="2295" windowWidth="27000" windowHeight="19635" xr2:uid="{0BDE95B1-4385-4AFA-974F-F26807504D5B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0BDE95B1-4385-4AFA-974F-F26807504D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>CONNECTICUT</t>
   </si>
   <si>
-    <t>DELEWARE</t>
-  </si>
-  <si>
     <t>DISTRICT OF COLUMBIA</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>WYOMING</t>
+  </si>
+  <si>
+    <t>DELAWARE</t>
   </si>
 </sst>
 </file>
@@ -221,7 +221,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0000_);\(#,##0.0000\)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000_);\(#,##0.0000\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -265,10 +265,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -290,9 +290,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -330,7 +330,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -436,7 +436,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -578,7 +578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,17 +588,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDB2D0BF-AB98-4C44-9E5D-9B435F1E12FF}">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -614,7 +614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -622,7 +622,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -630,7 +630,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -638,7 +638,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -646,7 +646,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -654,7 +654,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -662,7 +662,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -670,393 +670,393 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="B10" s="3">
         <v>0.79200000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3">
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>0.1426</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3">
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3">
         <v>8.4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3">
         <v>3.4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3">
         <v>2.4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3">
         <v>3.9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3">
         <v>4.3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3">
         <v>2.7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3">
         <v>3.6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3">
         <v>5.2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3">
         <v>2.7</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3">
         <v>3.8</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3">
         <v>3.3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3">
         <v>1.3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3">
         <v>1.7</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3">
         <v>0.75180000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3">
         <v>2.6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3">
         <v>10.1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3">
         <v>4.5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3">
         <v>1.8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3">
         <v>8.3299999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3">
         <v>6.6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="3">
         <v>2.9</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="3">
         <v>8.1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3">
         <v>0.99370000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="3">
         <v>1.3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="3">
         <v>3.7</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="3">
         <v>14.2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="3">
         <v>0.14829999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="3">
         <v>1.8</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="3">
         <v>0.85209999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="3">
         <v>4.5</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="3">
         <v>2.8</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="3">
         <v>2.2999999999999998</v>

</xml_diff>